<commit_message>
Notas do fórum para a semana 05/06/2022 a 11/06/2022 no semestre 20022-1
</commit_message>
<xml_diff>
--- a/build/ensino/2022/02/primeiro-semestre-de-2022/mes-5-dia-29-ava-matc65.xlsx
+++ b/build/ensino/2022/02/primeiro-semestre-de-2022/mes-5-dia-29-ava-matc65.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -400,20 +400,10 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>2022-06-05</t>
+          <t>total_views</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>2022-06-06</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>total_views</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>nota_view</t>
         </is>
@@ -452,12 +442,6 @@
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -487,15 +471,9 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>6</v>
-      </c>
-      <c r="L3">
         <v>2</v>
       </c>
     </row>
@@ -527,15 +505,9 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>9</v>
-      </c>
-      <c r="L4">
         <v>2</v>
       </c>
     </row>
@@ -572,12 +544,6 @@
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -607,15 +573,9 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
         <v>0.5</v>
       </c>
     </row>
@@ -652,12 +612,6 @@
       <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -687,15 +641,9 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
         <v>0.5</v>
       </c>
     </row>
@@ -732,12 +680,6 @@
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -772,12 +714,6 @@
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -807,15 +743,9 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
         <v>0.5</v>
       </c>
     </row>
@@ -847,15 +777,9 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>5</v>
-      </c>
-      <c r="L12">
         <v>2</v>
       </c>
     </row>
@@ -892,12 +816,6 @@
       <c r="J13">
         <v>0</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -927,15 +845,9 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
         <v>0.5</v>
       </c>
     </row>
@@ -972,12 +884,6 @@
       <c r="J15">
         <v>0</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1007,15 +913,9 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>7</v>
-      </c>
-      <c r="L16">
         <v>2</v>
       </c>
     </row>
@@ -1052,12 +952,6 @@
       <c r="J17">
         <v>0</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1087,16 +981,10 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>0</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>0.5</v>
       </c>
     </row>
     <row r="19">
@@ -1132,12 +1020,6 @@
       <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1172,12 +1054,6 @@
       <c r="J20">
         <v>0</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1212,12 +1088,6 @@
       <c r="J21">
         <v>0</v>
       </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1252,12 +1122,6 @@
       <c r="J22">
         <v>0</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1287,15 +1151,9 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23">
-        <v>7</v>
-      </c>
-      <c r="L23">
         <v>2</v>
       </c>
     </row>
@@ -1332,12 +1190,6 @@
       <c r="J24">
         <v>0</v>
       </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1372,12 +1224,6 @@
       <c r="J25">
         <v>0</v>
       </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1412,12 +1258,6 @@
       <c r="J26">
         <v>0</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1447,15 +1287,9 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>4</v>
-      </c>
-      <c r="L27">
         <v>2</v>
       </c>
     </row>
@@ -1492,12 +1326,6 @@
       <c r="J28">
         <v>0</v>
       </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1527,15 +1355,9 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>4</v>
-      </c>
-      <c r="L29">
         <v>2</v>
       </c>
     </row>
@@ -1572,12 +1394,6 @@
       <c r="J30">
         <v>0</v>
       </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1612,12 +1428,6 @@
       <c r="J31">
         <v>0</v>
       </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1652,12 +1462,6 @@
       <c r="J32">
         <v>0</v>
       </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1687,15 +1491,9 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33">
         <v>0.5</v>
       </c>
     </row>
@@ -1732,12 +1530,6 @@
       <c r="J34">
         <v>0</v>
       </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1767,15 +1559,9 @@
         <v>1</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J35">
-        <v>1</v>
-      </c>
-      <c r="K35">
-        <v>9</v>
-      </c>
-      <c r="L35">
         <v>2</v>
       </c>
     </row>
@@ -1812,12 +1598,6 @@
       <c r="J36">
         <v>0</v>
       </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1852,12 +1632,6 @@
       <c r="J37">
         <v>0</v>
       </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1892,12 +1666,6 @@
       <c r="J38">
         <v>0</v>
       </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1927,15 +1695,9 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>1</v>
-      </c>
-      <c r="L39">
         <v>0.5</v>
       </c>
     </row>
@@ -1972,12 +1734,6 @@
       <c r="J40">
         <v>0</v>
       </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2010,12 +1766,6 @@
         <v>1</v>
       </c>
       <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>2</v>
-      </c>
-      <c r="L41">
         <v>0.5</v>
       </c>
     </row>
@@ -2052,12 +1802,6 @@
       <c r="J42">
         <v>0</v>
       </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2087,15 +1831,9 @@
         <v>1</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
-        <v>7</v>
-      </c>
-      <c r="L43">
         <v>2</v>
       </c>
     </row>
@@ -2127,15 +1865,9 @@
         <v>1</v>
       </c>
       <c r="I44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J44">
-        <v>1</v>
-      </c>
-      <c r="K44">
-        <v>6</v>
-      </c>
-      <c r="L44">
         <v>2</v>
       </c>
     </row>
@@ -2172,12 +1904,6 @@
       <c r="J45">
         <v>0</v>
       </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2212,12 +1938,6 @@
       <c r="J46">
         <v>0</v>
       </c>
-      <c r="K46">
-        <v>0</v>
-      </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2250,12 +1970,6 @@
         <v>0</v>
       </c>
       <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
         <v>0</v>
       </c>
     </row>

</xml_diff>